<commit_message>
updated node.xlsx and clang.xlsx
</commit_message>
<xml_diff>
--- a/node.xlsx
+++ b/node.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xdong\OneDrive\Paper\git_hub\shared_ptp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/29e1f5b82a02f9e3/Paper/git_hub/shared_ptp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_48E8C9C14339E77D09F66B3321A9470AAD24B03A" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{AD471C79-3907-4FBE-88B3-82E87F6637A1}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_48E8C9C14339E77D09F66B3321A9470AAD24B03A" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B9D141A1-6A6B-45B1-805E-7A41CF4ABD98}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,13 +391,13 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="5" builtinId="3"/>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC9DE2B-F246-4FFD-B538-D1EE5E87FC9D}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -696,7 +696,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.65">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1116,7 +1116,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.65">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="18" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="8">
@@ -1191,7 +1191,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="8">
@@ -1208,20 +1208,20 @@
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8">
-        <f t="shared" ref="G28:G31" si="3">C28/B28</f>
+        <f t="shared" ref="G28:G29" si="3">C28/B28</f>
         <v>1.0163841927241251</v>
       </c>
       <c r="H28" s="8">
-        <f t="shared" ref="H28:H31" si="4">D28/B28</f>
+        <f t="shared" ref="H28:H29" si="4">D28/B28</f>
         <v>0.94458717724593089</v>
       </c>
       <c r="I28" s="8">
-        <f t="shared" ref="I28:I31" si="5">E28/B28</f>
+        <f t="shared" ref="I28:I29" si="5">E28/B28</f>
         <v>0.86527430811663408</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="8">
@@ -1251,33 +1251,33 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="20" t="s">
         <v>67</v>
       </c>
       <c r="B30" s="8">
-        <v>1029.3789999999999</v>
+        <v>530.93349999999998</v>
       </c>
       <c r="C30" s="8">
-        <v>1029.58</v>
+        <v>531.13049999999998</v>
       </c>
       <c r="D30" s="8">
-        <v>1015.258</v>
+        <v>525.99800000000005</v>
       </c>
       <c r="E30" s="8">
-        <v>1014.2805</v>
+        <v>524.89200000000005</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8">
         <f>C30/B30</f>
-        <v>1.0001952633578108</v>
+        <v>1.0003710445846796</v>
       </c>
       <c r="H30" s="8">
         <f>D30/B30</f>
-        <v>0.98628202051916747</v>
+        <v>0.99070410889499361</v>
       </c>
       <c r="I30" s="8">
         <f>E30/B30</f>
-        <v>0.98533241886613199</v>
+        <v>0.98862098549065014</v>
       </c>
     </row>
   </sheetData>
@@ -1303,11 +1303,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="10"/>
       <c r="F1" s="6"/>
     </row>
@@ -3110,18 +3110,18 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" s="2"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>

</xml_diff>